<commit_message>
Uren bijwerking referentiewaarde toegevoegt
</commit_message>
<xml_diff>
--- a/uren DAS.xlsx
+++ b/uren DAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiket\Desktop\DAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiket\Desktop\DAS\R studio\de-R-space\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3A9605-DC8D-4EBD-9DD8-F9C0D646D741}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C57FAE-6EBC-4912-9D94-C08E419F7B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="615" windowWidth="26190" windowHeight="14625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="-120" windowWidth="27675" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="21">
   <si>
     <t>Activiteit</t>
   </si>
@@ -92,7 +92,10 @@
     <t>verwerken dataset ernst met knime, feedback verwerken op dataset. SPSS, R studio workshop gevolgt. R geprogrameert.</t>
   </si>
   <si>
-    <t>Github opzetten, bespreken met Ernst en Jo over data opschoning</t>
+    <t>Github opzetten, bespreken met Ernst en Jo over data opschoning, verder R programeren</t>
+  </si>
+  <si>
+    <t>R Markdown programmeren, verslag verwerken</t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,6 +1277,9 @@
       </c>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
+      <c r="R18" s="22" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -1323,6 +1329,9 @@
       </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
+      <c r="R19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1342,17 +1351,18 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="J20" s="8">
+        <v>6</v>
+      </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
-      <c r="O20" s="9"/>
+      <c r="O20" s="9">
+        <v>4</v>
+      </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -1432,18 +1442,24 @@
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="G24" s="14">
+        <v>4</v>
+      </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
+      <c r="K24" s="14">
+        <v>2</v>
+      </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
+      <c r="M24" s="14">
+        <v>2</v>
+      </c>
       <c r="N24" s="14"/>
       <c r="O24" s="15"/>
       <c r="Q24" s="21">
         <f>SUM(B20:O24)</f>
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1493,6 +1509,9 @@
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
+      <c r="R26" s="22" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -1542,21 +1561,32 @@
       </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
+      <c r="R27" s="23" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
+      <c r="C28" s="8">
+        <v>5</v>
+      </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="H28" s="8">
+        <v>2</v>
+      </c>
       <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
+      <c r="J28" s="8">
+        <v>2</v>
+      </c>
+      <c r="K28" s="8">
+        <v>5</v>
+      </c>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
@@ -1612,7 +1642,9 @@
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="D31" s="11">
+        <v>2</v>
+      </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -1634,22 +1666,34 @@
         <v>11</v>
       </c>
       <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
+      <c r="C32" s="14">
+        <v>2</v>
+      </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
+      <c r="F32" s="14">
+        <v>2</v>
+      </c>
+      <c r="G32" s="14">
+        <v>4</v>
+      </c>
+      <c r="H32" s="14">
+        <v>1</v>
+      </c>
+      <c r="I32" s="14">
+        <v>2</v>
+      </c>
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
+      <c r="L32" s="14">
+        <v>4</v>
+      </c>
       <c r="M32" s="14"/>
       <c r="N32" s="14"/>
       <c r="O32" s="15"/>
       <c r="Q32" s="21">
         <f>SUM(B28:O32)</f>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>